<commit_message>
Tabelas e Diagrama de Gantt - Partes 2 e 3
</commit_message>
<xml_diff>
--- a/Trabalho 2/JP/Diagramas e Tabelas.xlsx
+++ b/Trabalho 2/JP/Diagramas e Tabelas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Diagramas" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
   <si>
     <t>t0</t>
   </si>
@@ -81,157 +81,67 @@
     <t>Parte 2</t>
   </si>
   <si>
-    <t>Parte 1</t>
-  </si>
-  <si>
     <t>Parte 3</t>
-  </si>
-  <si>
-    <t>r0</t>
-  </si>
-  <si>
-    <t>r1</t>
-  </si>
-  <si>
-    <t>r2</t>
-  </si>
-  <si>
-    <t>r3</t>
-  </si>
-  <si>
-    <t>r6</t>
-  </si>
-  <si>
-    <t>r5</t>
-  </si>
-  <si>
-    <t>r10</t>
-  </si>
-  <si>
-    <t>r11</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>Parte 5</t>
-  </si>
-  <si>
-    <t>r0_1</t>
-  </si>
-  <si>
-    <t>r0_2</t>
-  </si>
-  <si>
-    <t>r1_1</t>
-  </si>
-  <si>
-    <t>r1_2</t>
-  </si>
-  <si>
-    <t>r2_1</t>
-  </si>
-  <si>
-    <t>r2_2</t>
-  </si>
-  <si>
-    <t>r3_1</t>
-  </si>
-  <si>
-    <t>r3_2</t>
-  </si>
-  <si>
-    <t>r5_1</t>
-  </si>
-  <si>
-    <t>r5_2</t>
-  </si>
-  <si>
-    <t>r6_1</t>
-  </si>
-  <si>
-    <t>r6_2</t>
-  </si>
-  <si>
-    <t>r10_1</t>
-  </si>
-  <si>
-    <t>r10_2</t>
-  </si>
-  <si>
-    <t>r11_1</t>
-  </si>
-  <si>
-    <t>r11_2</t>
-  </si>
-  <si>
-    <t>vi_0</t>
-  </si>
-  <si>
-    <t>vi_6</t>
-  </si>
-  <si>
-    <t>v0_1</t>
-  </si>
-  <si>
-    <t>v0_2</t>
-  </si>
-  <si>
-    <t>v0_5</t>
-  </si>
-  <si>
-    <t>v1_2</t>
-  </si>
-  <si>
-    <t>v2_3</t>
-  </si>
-  <si>
-    <t>v5_3</t>
-  </si>
-  <si>
-    <t>v6_7</t>
-  </si>
-  <si>
-    <t>v6_10</t>
-  </si>
-  <si>
-    <t>v7_2</t>
-  </si>
-  <si>
-    <t>v7_5</t>
-  </si>
-  <si>
-    <t>v7_9</t>
-  </si>
-  <si>
-    <t>v10_5</t>
-  </si>
-  <si>
-    <t>v10_9</t>
-  </si>
-  <si>
-    <t>v10_11</t>
-  </si>
-  <si>
-    <t>v11_9</t>
-  </si>
-  <si>
-    <t>v5_6</t>
-  </si>
-  <si>
-    <t>v3_f</t>
-  </si>
-  <si>
-    <t>v5_f</t>
-  </si>
-  <si>
-    <t>v9_f</t>
   </si>
   <si>
     <t>t4</t>
   </si>
   <si>
     <t>t8</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>y2</t>
+  </si>
+  <si>
+    <t>y3</t>
+  </si>
+  <si>
+    <t>y4</t>
+  </si>
+  <si>
+    <t>y5</t>
+  </si>
+  <si>
+    <t>y6</t>
+  </si>
+  <si>
+    <t>y7</t>
+  </si>
+  <si>
+    <t>y8</t>
+  </si>
+  <si>
+    <t>y9</t>
+  </si>
+  <si>
+    <t>y10</t>
+  </si>
+  <si>
+    <t>y11</t>
+  </si>
+  <si>
+    <t>y12</t>
+  </si>
+  <si>
+    <t>y13</t>
+  </si>
+  <si>
+    <t>y14</t>
+  </si>
+  <si>
+    <t>y15</t>
+  </si>
+  <si>
+    <t>y16</t>
+  </si>
+  <si>
+    <t>y17</t>
+  </si>
+  <si>
+    <t>y18</t>
   </si>
 </sst>
 </file>
@@ -255,7 +165,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -278,65 +188,27 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -511,16 +383,16 @@
                   <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.0</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.0</c:v>
@@ -724,11 +596,11 @@
         </c:dLbls>
         <c:gapWidth val="79"/>
         <c:overlap val="100"/>
-        <c:axId val="-2118802896"/>
-        <c:axId val="2078547488"/>
+        <c:axId val="2132994192"/>
+        <c:axId val="2137895824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2118802896"/>
+        <c:axId val="2132994192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -785,7 +657,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2078547488"/>
+        <c:crossAx val="2137895824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -793,7 +665,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2078547488"/>
+        <c:axId val="2137895824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -849,7 +721,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2118802896"/>
+        <c:crossAx val="2132994192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1242,11 +1114,11 @@
         </c:dLbls>
         <c:gapWidth val="79"/>
         <c:overlap val="100"/>
-        <c:axId val="2078344592"/>
-        <c:axId val="2078348240"/>
+        <c:axId val="-2070402464"/>
+        <c:axId val="2137901392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2078344592"/>
+        <c:axId val="-2070402464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1303,7 +1175,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2078348240"/>
+        <c:crossAx val="2137901392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1311,7 +1183,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2078348240"/>
+        <c:axId val="2137901392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1367,7 +1239,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2078344592"/>
+        <c:crossAx val="-2070402464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1488,8 +1360,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2122260832"/>
-        <c:axId val="-2122254944"/>
+        <c:axId val="2137803344"/>
+        <c:axId val="2137809232"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -1587,11 +1459,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2122260832"/>
-        <c:axId val="-2122254944"/>
+        <c:axId val="2137803344"/>
+        <c:axId val="2137809232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2122260832"/>
+        <c:axId val="2137803344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1634,7 +1506,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2122254944"/>
+        <c:crossAx val="2137809232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1642,7 +1514,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122254944"/>
+        <c:axId val="2137809232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1707,7 +1579,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2122260832"/>
+        <c:crossAx val="2137803344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2100,11 +1972,11 @@
         </c:dLbls>
         <c:gapWidth val="79"/>
         <c:overlap val="100"/>
-        <c:axId val="-2122171840"/>
-        <c:axId val="-2122168192"/>
+        <c:axId val="2137719088"/>
+        <c:axId val="2137722736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2122171840"/>
+        <c:axId val="2137719088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2161,7 +2033,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2122168192"/>
+        <c:crossAx val="2137722736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2169,7 +2041,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122168192"/>
+        <c:axId val="2137722736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2225,7 +2097,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2122171840"/>
+        <c:crossAx val="2137719088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4885,7 +4757,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4935,6 +4807,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
+        <f>B2+C2</f>
         <v>4</v>
       </c>
       <c r="C3" s="1">
@@ -4955,7 +4828,8 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>11</v>
+        <f>MAX(B3+C3,B6+C6)</f>
+        <v>20</v>
       </c>
       <c r="C4" s="1">
         <v>7</v>
@@ -4975,7 +4849,8 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>18</v>
+        <f>MAX(B4+C4, B7+C7)</f>
+        <v>27</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -4992,9 +4867,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1">
+        <f>MAX(B2+C2, B9+C9)</f>
         <v>11</v>
       </c>
       <c r="C6" s="1">
@@ -5015,7 +4891,8 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>13</v>
+        <f>MAX(B6+C6, B10+C10)</f>
+        <v>20</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>
@@ -5055,6 +4932,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
+        <f>SUM(B8, C8)</f>
         <v>5</v>
       </c>
       <c r="C9" s="1">
@@ -5072,9 +4950,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1">
+        <f>MAX(B9+C9, B12+C12)</f>
         <v>13</v>
       </c>
       <c r="C10" s="1">
@@ -5095,6 +4974,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1">
+        <f>MAX(B10+C10, B13+C13)</f>
         <v>20</v>
       </c>
       <c r="C11" s="1">
@@ -5115,6 +4995,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1">
+        <f>SUM(B8, C8)</f>
         <v>5</v>
       </c>
       <c r="C12" s="1">
@@ -5126,6 +5007,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1">
+        <f>SUM(B12, C12)</f>
         <v>13</v>
       </c>
       <c r="C13" s="1">
@@ -5149,7 +5031,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>22</v>
       </c>
@@ -5166,7 +5048,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>21</v>
       </c>
@@ -5183,7 +5065,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>20</v>
       </c>
@@ -5200,7 +5082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -5217,7 +5099,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -5234,7 +5116,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>17</v>
       </c>
@@ -5251,7 +5133,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="J24" s="1" t="s">
         <v>8</v>
       </c>
@@ -5262,7 +5144,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="J25" s="1" t="s">
         <v>9</v>
       </c>
@@ -5273,7 +5155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="J26" s="1" t="s">
         <v>10</v>
       </c>
@@ -5284,7 +5166,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="J27" s="1" t="s">
         <v>11</v>
       </c>
@@ -5307,51 +5189,47 @@
   <dimension ref="A1:Q139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="5" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="5" t="s">
-        <v>18</v>
+      <c r="H2" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="2"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="4"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2"/>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
       <c r="E3" s="3" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F3" s="3">
         <v>0</v>
@@ -5364,793 +5242,621 @@
         <v>0</v>
       </c>
       <c r="J3" s="2"/>
-      <c r="K3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="L3" s="4">
-        <v>0</v>
-      </c>
-      <c r="M3" s="2"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="4">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4">
-        <v>5</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="4">
-        <v>4</v>
+      <c r="I4" s="3">
+        <v>7</v>
       </c>
       <c r="J4" s="2"/>
-      <c r="K4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" s="4">
-        <v>3.5</v>
-      </c>
-      <c r="M4" s="2"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="4">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="3">
         <v>0</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="4" t="s">
+      <c r="G5" s="2"/>
+      <c r="H5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="4">
-        <v>11</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="4">
-        <v>10</v>
+      <c r="I5" s="3">
+        <v>13</v>
       </c>
       <c r="J5" s="2"/>
-      <c r="K5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="L5" s="4">
-        <v>9.5</v>
-      </c>
-      <c r="M5" s="2"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="4">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="3">
         <v>0</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="4" t="s">
+      <c r="G6" s="2"/>
+      <c r="H6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="4">
+      <c r="I6" s="3">
         <v>20</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6" s="4">
-        <v>17</v>
-      </c>
       <c r="J6" s="2"/>
-      <c r="K6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L6" s="4">
-        <v>16.5</v>
-      </c>
-      <c r="M6" s="2"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="4">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="3">
         <v>0</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="4" t="s">
+      <c r="G7" s="2"/>
+      <c r="H7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="4">
-        <v>16</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>13</v>
       </c>
       <c r="J7" s="2"/>
-      <c r="K7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L7" s="4">
-        <v>12.5</v>
-      </c>
-      <c r="M7" s="2"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="4">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="3">
         <v>0</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="4" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="4">
+      <c r="I8" s="3">
         <v>0</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="4">
-        <v>0</v>
-      </c>
       <c r="J8" s="2"/>
-      <c r="K8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L8" s="4">
-        <v>0</v>
-      </c>
-      <c r="M8" s="2"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="4">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="3">
         <v>0</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="4" t="s">
+      <c r="G9" s="2"/>
+      <c r="H9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="4">
-        <v>5</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" s="4">
-        <v>4</v>
+      <c r="I9" s="3">
+        <v>7</v>
       </c>
       <c r="J9" s="2"/>
-      <c r="K9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L9" s="4">
-        <v>3.5</v>
-      </c>
-      <c r="M9" s="2"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="4">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="3">
         <v>0</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="4" t="s">
+      <c r="G10" s="2"/>
+      <c r="H10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="4">
+      <c r="I10" s="3">
         <v>20</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="4">
-        <v>17</v>
-      </c>
       <c r="J10" s="2"/>
-      <c r="K10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L10" s="4">
-        <v>16</v>
-      </c>
-      <c r="M10" s="2"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="4">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="3">
         <v>0</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="4" t="s">
+      <c r="G11" s="2"/>
+      <c r="H11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="4">
+      <c r="I11" s="3">
         <v>5</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="4">
-        <v>3</v>
-      </c>
       <c r="J11" s="2"/>
-      <c r="K11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L11" s="4">
-        <v>3</v>
-      </c>
-      <c r="M11" s="2"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="4">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="3">
         <v>0</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="4" t="s">
+      <c r="G12" s="2"/>
+      <c r="H12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="4">
+      <c r="I12" s="3">
         <v>13</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="4">
-        <v>11</v>
-      </c>
       <c r="J12" s="2"/>
-      <c r="K12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L12" s="4">
-        <v>10.5</v>
-      </c>
-      <c r="M12" s="2"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="4">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="4" t="s">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="4">
+      <c r="I13" s="3">
         <v>22</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="4">
-        <v>19</v>
-      </c>
       <c r="J13" s="2"/>
-      <c r="K13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L13" s="4">
-        <v>18</v>
-      </c>
-      <c r="M13" s="2"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="4">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="3">
         <v>0</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4">
+      <c r="G14" s="2"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3">
         <v>22</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" s="4">
-        <v>0</v>
-      </c>
       <c r="J14" s="2"/>
-      <c r="K14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="L14" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="M14" s="2"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="4">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
       <c r="G15" s="2"/>
-      <c r="H15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I15" s="4">
-        <v>0</v>
-      </c>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L15" s="4">
-        <v>0</v>
-      </c>
-      <c r="M15" s="2"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="4">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
       <c r="G16" s="2"/>
-      <c r="H16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I16" s="4">
-        <v>0</v>
-      </c>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L16" s="4">
-        <v>0</v>
-      </c>
-      <c r="M16" s="2"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="4">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
       <c r="G17" s="2"/>
-      <c r="H17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="4">
-        <v>0</v>
-      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="L17" s="4">
-        <v>0</v>
-      </c>
-      <c r="M17" s="2"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="4">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="3">
         <v>0</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I18" s="4">
-        <v>0</v>
-      </c>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L18" s="4">
-        <v>0</v>
-      </c>
-      <c r="M18" s="2"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="4">
-        <v>1</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
       <c r="G19" s="2"/>
-      <c r="H19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I19" s="4">
-        <v>2</v>
-      </c>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
       <c r="J19" s="2"/>
-      <c r="K19" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L19" s="4">
-        <v>0</v>
-      </c>
-      <c r="M19" s="2"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="4">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="3">
         <v>1</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I20" s="4">
-        <v>0</v>
-      </c>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L20" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="M20" s="2"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="4">
-        <v>0</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3">
+        <v>22</v>
+      </c>
       <c r="G21" s="2"/>
-      <c r="H21" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I21" s="4">
-        <v>1</v>
-      </c>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="L21" s="4">
-        <v>0</v>
-      </c>
-      <c r="M21" s="2"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="4">
-        <v>0</v>
-      </c>
-      <c r="D22" s="2"/>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I22" s="4">
-        <v>3</v>
-      </c>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="L22" s="4">
-        <v>0</v>
-      </c>
-      <c r="M22" s="2"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="4">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2"/>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="4">
-        <v>9580</v>
-      </c>
+      <c r="I23" s="4"/>
       <c r="J23" s="2"/>
-      <c r="K23" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="L23" s="4">
-        <v>0</v>
-      </c>
-      <c r="M23" s="2"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="4">
-        <v>22</v>
-      </c>
-      <c r="D24" s="2"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
-      <c r="K24" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L24" s="4">
-        <v>1</v>
-      </c>
-      <c r="M24" s="2"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
-      <c r="K25" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L25" s="4">
-        <v>1</v>
-      </c>
-      <c r="M25" s="2"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
-      <c r="K26" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L26" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="M26" s="2"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="L27" s="4">
-        <v>0</v>
-      </c>
-      <c r="M27" s="2"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
-      <c r="K28" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L28" s="4">
-        <v>1</v>
-      </c>
-      <c r="M28" s="2"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
-      <c r="K29" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="L29" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="M29" s="2"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -6160,19 +5866,15 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
-      <c r="K30" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L30" s="4">
-        <v>4</v>
-      </c>
-      <c r="M30" s="2"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -6183,16 +5885,14 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="4"/>
-      <c r="L31" s="4">
-        <v>19800</v>
-      </c>
-      <c r="M31" s="2"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -6202,9 +5902,9 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
@@ -6221,9 +5921,9 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>

</xml_diff>